<commit_message>
The new version of the tool using PaddleOCR
</commit_message>
<xml_diff>
--- a/CONFIG/lists.xlsx
+++ b/CONFIG/lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ELPV\ELPV_OCRTool\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EA4D3D-02FD-4DA3-9F9E-629017B5B47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D9BC4A-AD07-4428-A789-BD1E55431EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-12945" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,15 +118,9 @@
     <t>Espagne</t>
   </si>
   <si>
-    <t>Naccobus aberrans</t>
-  </si>
-  <si>
     <t>ALCMARIA</t>
   </si>
   <si>
-    <t>Italie</t>
-  </si>
-  <si>
     <t>PVY</t>
   </si>
   <si>
@@ -581,6 +575,12 @@
   </si>
   <si>
     <t>Imperativement garder les mêmes noms de colonnes</t>
+  </si>
+  <si>
+    <t>ALLIANS</t>
+  </si>
+  <si>
+    <t>Nacobbus aberrans</t>
   </si>
 </sst>
 </file>
@@ -599,6 +599,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -663,6 +664,20 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -680,20 +695,6 @@
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -708,9 +709,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}" name="Tableau1" displayName="Tableau1" ref="B1:B1048576" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}" name="Tableau1" displayName="Tableau1" ref="B1:B1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0" dataCellStyle="Normal">
   <autoFilter ref="B1:B1048576" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B156">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B157">
     <sortCondition ref="B1:B1048576"/>
   </sortState>
   <tableColumns count="1">
@@ -1005,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E156"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="T104" sqref="T104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1027,7 +1028,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1119,7 +1120,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -1130,763 +1131,765 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B139" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B140" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B141" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B152" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B154" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B155" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
-        <v>184</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B157" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the option of adding a new order manually on the interface and fix some bugs on the landscape format
</commit_message>
<xml_diff>
--- a/CONFIG/lists.xlsx
+++ b/CONFIG/lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ELPV\ELPV_OCRTool\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D9BC4A-AD07-4428-A789-BD1E55431EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CCD89F-7897-4480-AA2A-695F9550A2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12945" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="189">
   <si>
     <t>parasite</t>
   </si>
@@ -581,6 +581,12 @@
   </si>
   <si>
     <t>Nacobbus aberrans</t>
+  </si>
+  <si>
+    <t>LADY CLAIRE</t>
+  </si>
+  <si>
+    <t>SOPRANO</t>
   </si>
 </sst>
 </file>
@@ -1006,13 +1012,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E157"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1890,6 +1896,16 @@
     <row r="157" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B157" t="s">
         <v>182</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B158" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B159" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the name of copied samples
</commit_message>
<xml_diff>
--- a/CONFIG/lists.xlsx
+++ b/CONFIG/lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ELPV\ELPV_OCRTool\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09CCD89F-7897-4480-AA2A-695F9550A2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3324F8-2E85-4F85-BE23-320C05AF3BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="190">
   <si>
     <t>parasite</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>SOPRANO</t>
+  </si>
+  <si>
+    <t>Autoproduction</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1142,6 +1145,9 @@
       <c r="B9" t="s">
         <v>29</v>
       </c>
+      <c r="C9" t="s">
+        <v>189</v>
+      </c>
       <c r="D9" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Updated the eLIMS connectivity
</commit_message>
<xml_diff>
--- a/CONFIG/lists.xlsx
+++ b/CONFIG/lists.xlsx
@@ -8,22 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ELPV\ELPV_OCRTool\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3324F8-2E85-4F85-BE23-320C05AF3BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02A2988-846A-4BF1-9EC1-A320ECF55EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="lists" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="190">
-  <si>
-    <t>parasite</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
   <si>
     <t>variete</t>
   </si>
@@ -34,9 +31,6 @@
     <t>pays</t>
   </si>
   <si>
-    <t>Meloidogyne chitwoodi</t>
-  </si>
-  <si>
     <t>ACOUSTIC</t>
   </si>
   <si>
@@ -46,9 +40,6 @@
     <t>France</t>
   </si>
   <si>
-    <t>Meloidogyne fallax</t>
-  </si>
-  <si>
     <t>ADENA</t>
   </si>
   <si>
@@ -58,9 +49,6 @@
     <t>Pays Bas</t>
   </si>
   <si>
-    <t>Meloidogyne enterolobii</t>
-  </si>
-  <si>
     <t>ADORA</t>
   </si>
   <si>
@@ -70,9 +58,6 @@
     <t>Belgique</t>
   </si>
   <si>
-    <t>Ralstonia solanacearum</t>
-  </si>
-  <si>
     <t>AGATA</t>
   </si>
   <si>
@@ -82,9 +67,6 @@
     <t>Hollande</t>
   </si>
   <si>
-    <t>Clavibacter</t>
-  </si>
-  <si>
     <t>AGRIA</t>
   </si>
   <si>
@@ -94,9 +76,6 @@
     <t>Allemagne</t>
   </si>
   <si>
-    <t>Globodera pallida</t>
-  </si>
-  <si>
     <t>ALANIS</t>
   </si>
   <si>
@@ -106,9 +85,6 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>Globodera rostochiensis</t>
-  </si>
-  <si>
     <t>ALIANS</t>
   </si>
   <si>
@@ -121,27 +97,18 @@
     <t>ALCMARIA</t>
   </si>
   <si>
-    <t>PVY</t>
-  </si>
-  <si>
     <t>ALTESSE</t>
   </si>
   <si>
     <t>Suisse</t>
   </si>
   <si>
-    <t>Jambe noire</t>
-  </si>
-  <si>
     <t>ALOUETTE</t>
   </si>
   <si>
     <t>Pays-Bas</t>
   </si>
   <si>
-    <t>PLRV</t>
-  </si>
-  <si>
     <t>AMANDINE</t>
   </si>
   <si>
@@ -578,9 +545,6 @@
   </si>
   <si>
     <t>ALLIANS</t>
-  </si>
-  <si>
-    <t>Nacobbus aberrans</t>
   </si>
   <si>
     <t>LADY CLAIRE</t>
@@ -718,10 +682,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}" name="Tableau1" displayName="Tableau1" ref="B1:B1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0" dataCellStyle="Normal">
-  <autoFilter ref="B1:B1048576" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B157">
-    <sortCondition ref="B1:B1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}" name="Tableau1" displayName="Tableau1" ref="A1:A1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0" dataCellStyle="Normal">
+  <autoFilter ref="A1:A1048576" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A157">
+    <sortCondition ref="A1:A1048576"/>
   </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{34CC5E21-2539-4762-B392-1577EB39AB9E}" name="variete" dataCellStyle="Normal"/>
@@ -1015,903 +979,867 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:D159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>189</v>
-      </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>185</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B40" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B69" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B70" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B71" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B72" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B73" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B74" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B76" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B77" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B78" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B79" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B80" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B81" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B82" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B83" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B84" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B85" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B86" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B87" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B88" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B89" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B90" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B91" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B92" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B93" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B94" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B95" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B96" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B97" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B98" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B99" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B100" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B101" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B102" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B103" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B104" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B105" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B106" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B107" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B108" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B109" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B110" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B111" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B112" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B113" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B114" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B115" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B116" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B117" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B118" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B119" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B120" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B121" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B122" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B123" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B124" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B125" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B126" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B127" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B128" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B129" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B130" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B131" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B132" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B133" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B134" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B135" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B136" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B137" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B138" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B139" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B140" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B141" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B142" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B143" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B144" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B145" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B146" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B147" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B148" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B149" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B150" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B151" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B152" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B153" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B154" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B155" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B156" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B157" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B158" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B159" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more features to the SEMAE model, ability to copy last inputs and fixed dots detection
</commit_message>
<xml_diff>
--- a/CONFIG/lists.xlsx
+++ b/CONFIG/lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ELPV\ELPV_OCRTool\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02A2988-846A-4BF1-9EC1-A320ECF55EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C6FA5-9772-4975-8671-DD561F76E0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="184">
   <si>
     <t>variete</t>
   </si>
@@ -554,6 +554,24 @@
   </si>
   <si>
     <t>Autoproduction</t>
+  </si>
+  <si>
+    <t>OPAL</t>
+  </si>
+  <si>
+    <t>ENDURO</t>
+  </si>
+  <si>
+    <t>CORINNA</t>
+  </si>
+  <si>
+    <t>SH C 1010</t>
+  </si>
+  <si>
+    <t>RISSOLETTO</t>
+  </si>
+  <si>
+    <t>ASTERIX</t>
   </si>
 </sst>
 </file>
@@ -684,7 +702,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}" name="Tableau1" displayName="Tableau1" ref="A1:A1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0" dataCellStyle="Normal">
   <autoFilter ref="A1:A1048576" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A157">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A164">
     <sortCondition ref="A1:A1048576"/>
   </sortState>
   <tableColumns count="1">
@@ -979,13 +997,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D159"/>
+  <dimension ref="A1:D165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A165" sqref="A165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
@@ -1284,562 +1302,592 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>104</v>
+        <v>175</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>135</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>176</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added extension safety for pdf registration. Added a save for XMLs
</commit_message>
<xml_diff>
--- a/CONFIG/lists.xlsx
+++ b/CONFIG/lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CF6P\Desktop\ELPV\ELPV_OCRTool\CONFIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C6FA5-9772-4975-8671-DD561F76E0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57A9389-7334-4342-834D-BA0A85C7B0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4780" yWindow="850" windowWidth="14400" windowHeight="7370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lists" sheetId="1" r:id="rId1"/>
@@ -700,10 +700,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}" name="Tableau1" displayName="Tableau1" ref="A1:A1048576" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0" dataCellStyle="Normal">
-  <autoFilter ref="A1:A1048576" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A164">
-    <sortCondition ref="A1:A1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}" name="Tableau1" displayName="Tableau1" ref="A1:A1048575" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0" dataCellStyle="Normal">
+  <autoFilter ref="A1:A1048575" xr:uid="{31C349CA-A78E-41A8-8B37-697DF492EE93}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A165">
+    <sortCondition ref="A1:A1048575"/>
   </sortState>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{34CC5E21-2539-4762-B392-1577EB39AB9E}" name="variete" dataCellStyle="Normal"/>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A165" sqref="A165"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1167,657 +1167,657 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>179</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>101</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>178</v>
+        <v>131</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.35">
@@ -1827,67 +1827,67 @@
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>